<commit_message>
refactored, added postprocessor, readme
</commit_message>
<xml_diff>
--- a/speakers.xlsx
+++ b/speakers.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/riesbeck/workspace/javascript/vue/xls-vue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812FAA60-B2CE-CD49-9093-345C45B78020}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8327F259-2CAF-B948-8493-832FCCFB2D1F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="460" windowWidth="24540" windowHeight="15000" xr2:uid="{4EFB574D-799A-174D-9466-FBE510CC2F58}"/>
   </bookViews>
   <sheets>
-    <sheet name="speakers" sheetId="1" r:id="rId1"/>
+    <sheet name="Speakers" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,40 +32,40 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>image</t>
-  </si>
-  <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>Andy diSessa</t>
-  </si>
-  <si>
-    <t>andy.jpg</t>
-  </si>
-  <si>
-    <t>https://gse.berkeley.edu/andrea-disessa</t>
-  </si>
-  <si>
-    <t>Student models of behavior</t>
-  </si>
-  <si>
-    <t>Jane Kolodner</t>
-  </si>
-  <si>
-    <t>jk.jpg</t>
-  </si>
-  <si>
-    <t>https://www.bc.edu/bc-web/schools/lsoe/faculty-research/faculty-directory/janet-kolodner.html</t>
-  </si>
-  <si>
-    <t>Creativity</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Emily Dickinson</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Emily_Dickinson</t>
+  </si>
+  <si>
+    <t>Success is counted sweetest</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Gerard_Manley_Hopkins</t>
+  </si>
+  <si>
+    <t>Gerard Manley Hopkins</t>
+  </si>
+  <si>
+    <t>gmh.jpg</t>
+  </si>
+  <si>
+    <t>ed.png</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>Url</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>The Windhover</t>
   </si>
 </sst>
 </file>
@@ -101,8 +101,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,7 +421,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -433,38 +434,38 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>

</xml_diff>